<commit_message>
Adding script and loops to go through psychopy data and get differences between triggers, photodiodes, and stimuli; started on getting time differences between trials using loops to reorganize the data
</commit_message>
<xml_diff>
--- a/PsychoPyData_EEGMCT_ColumnKey.xlsx
+++ b/PsychoPyData_EEGMCT_ColumnKey.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uofc-my.sharepoint.com/personal/chelsie_hart_ucalgary_ca/Documents/1_PhD_Project/Scripting/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3277" documentId="8_{447AABAE-0265-45CA-9969-8E24E37FF3D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8A547B6B-13B5-445F-9D63-39C1C4FCD832}"/>
+  <xr:revisionPtr revIDLastSave="3285" documentId="8_{447AABAE-0265-45CA-9969-8E24E37FF3D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6119840B-AC81-43D8-BCAF-C5AB7391584D}"/>
   <bookViews>
-    <workbookView xWindow="-29530" yWindow="5130" windowWidth="28620" windowHeight="14870" xr2:uid="{5015AFB7-EBCA-4E4E-B1B8-96F1F0B54514}"/>
+    <workbookView xWindow="-19570" yWindow="1750" windowWidth="19380" windowHeight="18080" xr2:uid="{5015AFB7-EBCA-4E4E-B1B8-96F1F0B54514}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1333" uniqueCount="624">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1333" uniqueCount="625">
   <si>
     <t>date</t>
   </si>
@@ -1637,9 +1637,6 @@
     <t>PTrialToneStop</t>
   </si>
   <si>
-    <t>SoundTextToneStop</t>
-  </si>
-  <si>
     <t>TrialToneStop</t>
   </si>
   <si>
@@ -1908,6 +1905,12 @@
   </si>
   <si>
     <t>SoundTest_sound.stopped</t>
+  </si>
+  <si>
+    <t>SoundTestToneStop</t>
+  </si>
+  <si>
+    <t>Time since the start of the ROUTINE</t>
   </si>
 </sst>
 </file>
@@ -2065,23 +2068,120 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="19">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -2481,11 +2581,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{071F2C75-EFE1-4D36-A5E8-DE0C4083E759}">
   <dimension ref="A1:L342"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C54" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="G145" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E153" sqref="E153"/>
+      <selection pane="bottomRight" activeCell="H82" sqref="H82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2505,7 +2605,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="B1" t="s">
         <v>68</v>
@@ -2520,7 +2620,7 @@
         <v>506</v>
       </c>
       <c r="F1" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="G1" t="s">
         <v>54</v>
@@ -2535,7 +2635,7 @@
         <v>122</v>
       </c>
       <c r="K1" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
@@ -2646,7 +2746,7 @@
       <c r="B7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="22"/>
+      <c r="D7" s="20"/>
       <c r="E7" s="10" t="s">
         <v>4</v>
       </c>
@@ -2664,7 +2764,7 @@
       <c r="B8" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="23" t="s">
+      <c r="D8" s="21" t="s">
         <v>439</v>
       </c>
       <c r="F8" t="s">
@@ -2680,7 +2780,7 @@
         <v>415</v>
       </c>
       <c r="K8" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
@@ -2843,7 +2943,7 @@
         <v>437</v>
       </c>
       <c r="K20" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.35">
@@ -2904,7 +3004,7 @@
         <v>434</v>
       </c>
       <c r="K24" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.35">
@@ -3019,7 +3119,7 @@
         <v>435</v>
       </c>
       <c r="K32" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.35">
@@ -3133,7 +3233,7 @@
         <v>453</v>
       </c>
       <c r="K40" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="41" spans="2:11" x14ac:dyDescent="0.35">
@@ -3163,7 +3263,7 @@
         <v>450</v>
       </c>
       <c r="K42" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="43" spans="2:11" x14ac:dyDescent="0.35">
@@ -3279,7 +3379,7 @@
         <v>147</v>
       </c>
       <c r="B52" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="D52" s="18"/>
       <c r="G52" t="s">
@@ -3294,7 +3394,7 @@
         <v>148</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="D53" s="19"/>
       <c r="E53" s="11"/>
@@ -3310,7 +3410,7 @@
         <v>150</v>
       </c>
       <c r="B54" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="D54" s="17" t="s">
         <v>448</v>
@@ -3325,7 +3425,7 @@
         <v>450</v>
       </c>
       <c r="K54" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.35">
@@ -3333,7 +3433,7 @@
         <v>151</v>
       </c>
       <c r="B55" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="D55" s="18"/>
       <c r="E55" s="8" t="s">
@@ -3346,7 +3446,7 @@
         <v>450</v>
       </c>
       <c r="K55" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.35">
@@ -3354,7 +3454,7 @@
         <v>152</v>
       </c>
       <c r="B56" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="D56" s="18"/>
       <c r="G56" t="s">
@@ -3379,7 +3479,7 @@
         <v>450</v>
       </c>
       <c r="K57" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.35">
@@ -3492,11 +3592,11 @@
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B67" s="6" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="D67" s="18"/>
       <c r="E67" s="8" t="s">
-        <v>533</v>
+        <v>623</v>
       </c>
       <c r="G67" t="s">
         <v>449</v>
@@ -3508,7 +3608,7 @@
         <v>438</v>
       </c>
       <c r="K67" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.35">
@@ -3516,7 +3616,7 @@
         <v>162</v>
       </c>
       <c r="B68" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="D68" s="18"/>
       <c r="G68" t="s">
@@ -3531,7 +3631,7 @@
         <v>163</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="D69" s="19"/>
       <c r="E69" s="11"/>
@@ -3539,7 +3639,7 @@
         <v>449</v>
       </c>
       <c r="H69" s="3" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.35">
@@ -3565,7 +3665,7 @@
         <v>481</v>
       </c>
       <c r="K70" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.35">
@@ -3583,7 +3683,7 @@
         <v>450</v>
       </c>
       <c r="K71" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.35">
@@ -3613,7 +3713,7 @@
         <v>450</v>
       </c>
       <c r="K73" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.35">
@@ -3730,13 +3830,13 @@
         <v>449</v>
       </c>
       <c r="H82" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="I82" t="s">
         <v>456</v>
       </c>
       <c r="K82" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="83" spans="2:11" x14ac:dyDescent="0.35">
@@ -3754,13 +3854,13 @@
         <v>449</v>
       </c>
       <c r="H83" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="I83" t="s">
         <v>488</v>
       </c>
       <c r="K83" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="84" spans="2:11" x14ac:dyDescent="0.35">
@@ -3775,10 +3875,10 @@
         <v>449</v>
       </c>
       <c r="H84" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="K84" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="85" spans="2:11" x14ac:dyDescent="0.35">
@@ -3805,10 +3905,10 @@
         <v>449</v>
       </c>
       <c r="H86" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="K86" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="87" spans="2:11" x14ac:dyDescent="0.35">
@@ -3838,7 +3938,7 @@
         <v>450</v>
       </c>
       <c r="K88" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="89" spans="2:11" x14ac:dyDescent="0.35">
@@ -3869,13 +3969,13 @@
       <c r="B91" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D91" s="20"/>
+      <c r="D91" s="22"/>
       <c r="E91" s="13"/>
       <c r="G91" s="7" t="s">
         <v>449</v>
       </c>
       <c r="H91" s="7" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="I91" s="7" t="s">
         <v>486</v>
@@ -3885,7 +3985,7 @@
       <c r="B92" t="s">
         <v>5</v>
       </c>
-      <c r="D92" s="21" t="s">
+      <c r="D92" s="23" t="s">
         <v>464</v>
       </c>
       <c r="F92" t="s">
@@ -3901,7 +4001,7 @@
         <v>460</v>
       </c>
       <c r="K92" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="93" spans="2:11" x14ac:dyDescent="0.35">
@@ -3919,7 +4019,7 @@
         <v>75</v>
       </c>
       <c r="K93" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="94" spans="2:11" x14ac:dyDescent="0.35">
@@ -3941,7 +4041,7 @@
       <c r="B95" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D95" s="20"/>
+      <c r="D95" s="22"/>
       <c r="E95" s="13"/>
       <c r="F95" s="7" t="s">
         <v>84</v>
@@ -3956,7 +4056,7 @@
         <v>117</v>
       </c>
       <c r="K95" s="7" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="96" spans="2:11" x14ac:dyDescent="0.35">
@@ -3966,7 +4066,7 @@
       <c r="C96" t="s">
         <v>417</v>
       </c>
-      <c r="D96" s="21" t="s">
+      <c r="D96" s="23" t="s">
         <v>465</v>
       </c>
       <c r="E96" s="8" t="s">
@@ -3982,7 +4082,7 @@
         <v>430</v>
       </c>
       <c r="K96" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="97" spans="2:12" x14ac:dyDescent="0.35">
@@ -4024,7 +4124,7 @@
         <v>430</v>
       </c>
       <c r="K98" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="99" spans="2:12" x14ac:dyDescent="0.35">
@@ -4124,7 +4224,7 @@
         <v>475</v>
       </c>
       <c r="K103" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="104" spans="2:12" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -4143,13 +4243,13 @@
         <v>449</v>
       </c>
       <c r="H104" s="3" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="I104" s="3" t="s">
         <v>430</v>
       </c>
       <c r="K104" s="3" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="105" spans="2:12" x14ac:dyDescent="0.35">
@@ -4169,7 +4269,7 @@
         <v>450</v>
       </c>
       <c r="K105" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="106" spans="2:12" x14ac:dyDescent="0.35">
@@ -4199,7 +4299,7 @@
         <v>450</v>
       </c>
       <c r="K107" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="108" spans="2:12" x14ac:dyDescent="0.35">
@@ -4269,7 +4369,7 @@
         <v>120</v>
       </c>
       <c r="K112" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="113" spans="2:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -4285,10 +4385,10 @@
         <v>449</v>
       </c>
       <c r="H113" s="3" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="K113" s="3" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="114" spans="2:11" x14ac:dyDescent="0.35">
@@ -4308,7 +4408,7 @@
         <v>450</v>
       </c>
       <c r="K114" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="115" spans="2:11" x14ac:dyDescent="0.35">
@@ -4338,7 +4438,7 @@
         <v>450</v>
       </c>
       <c r="K116" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="117" spans="2:11" x14ac:dyDescent="0.35">
@@ -4408,7 +4508,7 @@
         <v>118</v>
       </c>
       <c r="K121" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="122" spans="2:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -4424,10 +4524,10 @@
         <v>449</v>
       </c>
       <c r="H122" s="3" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="K122" s="3" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="123" spans="2:11" x14ac:dyDescent="0.35">
@@ -4453,7 +4553,7 @@
         <v>430</v>
       </c>
       <c r="K123" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="124" spans="2:11" x14ac:dyDescent="0.35">
@@ -4495,7 +4595,7 @@
         <v>430</v>
       </c>
       <c r="K125" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="126" spans="2:11" x14ac:dyDescent="0.35">
@@ -4592,7 +4692,7 @@
         <v>489</v>
       </c>
       <c r="K130" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="131" spans="2:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -4611,13 +4711,13 @@
         <v>449</v>
       </c>
       <c r="H131" s="3" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="I131" s="3" t="s">
         <v>430</v>
       </c>
       <c r="K131" s="3" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="132" spans="2:11" x14ac:dyDescent="0.35">
@@ -4637,7 +4737,7 @@
         <v>450</v>
       </c>
       <c r="K132" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="133" spans="2:11" x14ac:dyDescent="0.35">
@@ -4667,7 +4767,7 @@
         <v>450</v>
       </c>
       <c r="K134" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="135" spans="2:11" x14ac:dyDescent="0.35">
@@ -4700,7 +4800,7 @@
       </c>
       <c r="D137" s="18"/>
       <c r="G137" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="H137" t="s">
         <v>477</v>
@@ -4719,13 +4819,13 @@
         <v>449</v>
       </c>
       <c r="H138" s="3" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="I138" s="3" t="s">
         <v>478</v>
       </c>
       <c r="K138" s="3" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="139" spans="2:11" x14ac:dyDescent="0.35">
@@ -4751,7 +4851,7 @@
         <v>482</v>
       </c>
       <c r="K139" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="140" spans="2:11" x14ac:dyDescent="0.35">
@@ -4769,7 +4869,7 @@
         <v>450</v>
       </c>
       <c r="K140" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="141" spans="2:11" x14ac:dyDescent="0.35">
@@ -4799,7 +4899,7 @@
         <v>450</v>
       </c>
       <c r="K142" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="143" spans="2:11" x14ac:dyDescent="0.35">
@@ -4898,7 +4998,7 @@
         <v>456</v>
       </c>
       <c r="K149" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="150" spans="1:11" x14ac:dyDescent="0.35">
@@ -4907,7 +5007,7 @@
       </c>
       <c r="D150" s="18"/>
       <c r="E150" s="8" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="F150" t="s">
         <v>484</v>
@@ -4922,7 +5022,7 @@
         <v>488</v>
       </c>
       <c r="K150" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="151" spans="1:11" x14ac:dyDescent="0.35">
@@ -4930,11 +5030,11 @@
         <v>232</v>
       </c>
       <c r="B151" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="D151" s="18"/>
       <c r="E151" s="8" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="G151" t="s">
         <v>449</v>
@@ -4943,7 +5043,7 @@
         <v>450</v>
       </c>
       <c r="K151" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="152" spans="1:11" x14ac:dyDescent="0.35">
@@ -4951,7 +5051,7 @@
         <v>234</v>
       </c>
       <c r="B152" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="D152" s="18"/>
       <c r="G152" t="s">
@@ -4967,7 +5067,7 @@
       </c>
       <c r="D153" s="18"/>
       <c r="E153" s="8" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="G153" t="s">
         <v>449</v>
@@ -4976,7 +5076,7 @@
         <v>450</v>
       </c>
       <c r="K153" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="154" spans="1:11" x14ac:dyDescent="0.35">
@@ -5006,7 +5106,7 @@
         <v>450</v>
       </c>
       <c r="K155" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="156" spans="1:11" x14ac:dyDescent="0.35">
@@ -5043,7 +5143,7 @@
         <v>449</v>
       </c>
       <c r="H158" s="3" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="I158" s="3" t="s">
         <v>487</v>
@@ -5057,7 +5157,7 @@
         <v>490</v>
       </c>
       <c r="E159" s="8" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G159" t="s">
         <v>449</v>
@@ -5069,7 +5169,7 @@
         <v>430</v>
       </c>
       <c r="K159" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="160" spans="1:11" x14ac:dyDescent="0.35">
@@ -5093,7 +5193,7 @@
       </c>
       <c r="D161" s="18"/>
       <c r="E161" s="8" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="G161" t="s">
         <v>449</v>
@@ -5105,7 +5205,7 @@
         <v>430</v>
       </c>
       <c r="K161" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="162" spans="2:11" x14ac:dyDescent="0.35">
@@ -5187,7 +5287,7 @@
         <v>475</v>
       </c>
       <c r="K166" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="167" spans="2:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -5203,13 +5303,13 @@
         <v>449</v>
       </c>
       <c r="H167" s="3" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="I167" s="3" t="s">
         <v>430</v>
       </c>
       <c r="K167" s="3" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="168" spans="2:11" x14ac:dyDescent="0.35">
@@ -5220,16 +5320,16 @@
         <v>491</v>
       </c>
       <c r="E168" s="8" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="G168" t="s">
         <v>449</v>
       </c>
-      <c r="H168" t="s">
-        <v>450</v>
+      <c r="H168" s="2" t="s">
+        <v>624</v>
       </c>
       <c r="K168" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="169" spans="2:11" x14ac:dyDescent="0.35">
@@ -5240,8 +5340,8 @@
       <c r="G169" t="s">
         <v>449</v>
       </c>
-      <c r="H169" t="s">
-        <v>450</v>
+      <c r="H169" s="2" t="s">
+        <v>624</v>
       </c>
     </row>
     <row r="170" spans="2:11" x14ac:dyDescent="0.35">
@@ -5250,7 +5350,7 @@
       </c>
       <c r="D170" s="18"/>
       <c r="E170" s="8" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="G170" t="s">
         <v>449</v>
@@ -5259,7 +5359,7 @@
         <v>450</v>
       </c>
       <c r="K170" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="171" spans="2:11" x14ac:dyDescent="0.35">
@@ -5329,7 +5429,7 @@
         <v>120</v>
       </c>
       <c r="K175" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="176" spans="2:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -5345,10 +5445,10 @@
         <v>449</v>
       </c>
       <c r="H176" s="3" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="K176" s="3" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="177" spans="2:11" x14ac:dyDescent="0.35">
@@ -5359,16 +5459,16 @@
         <v>492</v>
       </c>
       <c r="E177" s="8" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="G177" t="s">
         <v>449</v>
       </c>
-      <c r="H177" t="s">
-        <v>450</v>
+      <c r="H177" s="2" t="s">
+        <v>624</v>
       </c>
       <c r="K177" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="178" spans="2:11" x14ac:dyDescent="0.35">
@@ -5379,8 +5479,8 @@
       <c r="G178" t="s">
         <v>449</v>
       </c>
-      <c r="H178" t="s">
-        <v>450</v>
+      <c r="H178" s="2" t="s">
+        <v>624</v>
       </c>
     </row>
     <row r="179" spans="2:11" x14ac:dyDescent="0.35">
@@ -5389,7 +5489,7 @@
       </c>
       <c r="D179" s="18"/>
       <c r="E179" s="8" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="G179" t="s">
         <v>449</v>
@@ -5398,7 +5498,7 @@
         <v>450</v>
       </c>
       <c r="K179" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="180" spans="2:11" x14ac:dyDescent="0.35">
@@ -5468,7 +5568,7 @@
         <v>118</v>
       </c>
       <c r="K184" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="185" spans="2:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -5484,10 +5584,10 @@
         <v>449</v>
       </c>
       <c r="H185" s="3" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="K185" s="3" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="186" spans="2:11" x14ac:dyDescent="0.35">
@@ -5498,7 +5598,7 @@
         <v>493</v>
       </c>
       <c r="E186" s="8" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="G186" t="s">
         <v>449</v>
@@ -5507,7 +5607,7 @@
         <v>450</v>
       </c>
       <c r="K186" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="187" spans="2:11" x14ac:dyDescent="0.35">
@@ -5528,7 +5628,7 @@
       </c>
       <c r="D188" s="18"/>
       <c r="E188" s="8" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="G188" t="s">
         <v>449</v>
@@ -5537,7 +5637,7 @@
         <v>450</v>
       </c>
       <c r="K188" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="189" spans="2:11" x14ac:dyDescent="0.35">
@@ -5607,7 +5707,7 @@
         <v>500</v>
       </c>
       <c r="K193" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="194" spans="2:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -5623,10 +5723,10 @@
         <v>449</v>
       </c>
       <c r="H194" s="3" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="K194" s="3" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="195" spans="2:11" x14ac:dyDescent="0.35">
@@ -5637,7 +5737,7 @@
         <v>499</v>
       </c>
       <c r="E195" s="8" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="F195" t="s">
         <v>501</v>
@@ -5649,7 +5749,7 @@
         <v>450</v>
       </c>
       <c r="K195" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="196" spans="2:11" x14ac:dyDescent="0.35">
@@ -5670,19 +5770,19 @@
       </c>
       <c r="D197" s="18"/>
       <c r="E197" s="11" t="s">
+        <v>544</v>
+      </c>
+      <c r="G197" s="3" t="s">
+        <v>449</v>
+      </c>
+      <c r="H197" s="3" t="s">
+        <v>450</v>
+      </c>
+      <c r="I197" s="3" t="s">
         <v>545</v>
       </c>
-      <c r="G197" s="3" t="s">
-        <v>449</v>
-      </c>
-      <c r="H197" s="3" t="s">
-        <v>450</v>
-      </c>
-      <c r="I197" s="3" t="s">
-        <v>546</v>
-      </c>
       <c r="K197" s="3" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="198" spans="2:11" x14ac:dyDescent="0.35">
@@ -5725,13 +5825,13 @@
         <v>449</v>
       </c>
       <c r="H200" s="3" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="I200" s="3" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="K200" s="3" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="201" spans="2:11" x14ac:dyDescent="0.35">
@@ -5739,13 +5839,13 @@
         <v>274</v>
       </c>
       <c r="D201" s="17" t="s">
+        <v>547</v>
+      </c>
+      <c r="E201" s="8" t="s">
         <v>548</v>
       </c>
-      <c r="E201" s="8" t="s">
-        <v>549</v>
-      </c>
       <c r="F201" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="G201" t="s">
         <v>449</v>
@@ -5754,7 +5854,7 @@
         <v>450</v>
       </c>
       <c r="K201" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="202" spans="2:11" x14ac:dyDescent="0.35">
@@ -5775,7 +5875,7 @@
       </c>
       <c r="D203" s="18"/>
       <c r="E203" s="8" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="G203" t="s">
         <v>449</v>
@@ -5784,7 +5884,7 @@
         <v>450</v>
       </c>
       <c r="K203" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="204" spans="2:11" x14ac:dyDescent="0.35">
@@ -5941,7 +6041,7 @@
         <v>70</v>
       </c>
       <c r="H216" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="217" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -5951,39 +6051,39 @@
       <c r="D217" s="19"/>
       <c r="E217" s="11"/>
       <c r="F217" s="3" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="G217" s="3" t="s">
         <v>449</v>
       </c>
       <c r="H217" s="3" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="I217" s="3" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="K217" s="3" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="218" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="C218" s="14" t="s">
+        <v>595</v>
+      </c>
+      <c r="D218" s="15" t="s">
         <v>596</v>
       </c>
-      <c r="D218" s="15" t="s">
+      <c r="E218" s="16" t="s">
         <v>597</v>
       </c>
-      <c r="E218" s="16" t="s">
+      <c r="F218" s="14" t="s">
         <v>598</v>
       </c>
-      <c r="F218" s="14" t="s">
+      <c r="G218" s="14" t="s">
         <v>599</v>
       </c>
-      <c r="G218" s="14" t="s">
+      <c r="H218" s="14" t="s">
         <v>600</v>
-      </c>
-      <c r="H218" s="14" t="s">
-        <v>601</v>
       </c>
     </row>
     <row r="219" spans="1:11" x14ac:dyDescent="0.35">
@@ -5991,13 +6091,13 @@
         <v>290</v>
       </c>
       <c r="D219" s="17" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E219" s="8" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="F219" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="G219" t="s">
         <v>449</v>
@@ -6006,7 +6106,7 @@
         <v>450</v>
       </c>
       <c r="K219" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="220" spans="1:11" x14ac:dyDescent="0.35">
@@ -6027,7 +6127,7 @@
       </c>
       <c r="D221" s="18"/>
       <c r="E221" s="8" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="G221" t="s">
         <v>449</v>
@@ -6036,7 +6136,7 @@
         <v>450</v>
       </c>
       <c r="K221" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="222" spans="1:11" x14ac:dyDescent="0.35">
@@ -6129,10 +6229,10 @@
         <v>300</v>
       </c>
       <c r="D229" s="17" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="E229" s="8" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="G229" t="s">
         <v>449</v>
@@ -6141,7 +6241,7 @@
         <v>450</v>
       </c>
       <c r="K229" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="230" spans="1:11" x14ac:dyDescent="0.35">
@@ -6162,7 +6262,7 @@
       </c>
       <c r="D231" s="18"/>
       <c r="E231" s="8" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="G231" t="s">
         <v>449</v>
@@ -6171,7 +6271,7 @@
         <v>450</v>
       </c>
       <c r="K231" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="232" spans="1:11" x14ac:dyDescent="0.35">
@@ -6216,10 +6316,10 @@
         <v>306</v>
       </c>
       <c r="D235" s="17" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="E235" s="8" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="G235" t="s">
         <v>449</v>
@@ -6228,7 +6328,7 @@
         <v>450</v>
       </c>
       <c r="K235" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="236" spans="1:11" x14ac:dyDescent="0.35">
@@ -6249,7 +6349,7 @@
       </c>
       <c r="D237" s="18"/>
       <c r="E237" s="8" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="G237" t="s">
         <v>449</v>
@@ -6258,7 +6358,7 @@
         <v>450</v>
       </c>
       <c r="K237" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="238" spans="1:11" x14ac:dyDescent="0.35">
@@ -6366,7 +6466,7 @@
         <v>70</v>
       </c>
       <c r="H246" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="247" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -6379,7 +6479,7 @@
         <v>449</v>
       </c>
       <c r="H247" s="3" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="248" spans="1:11" x14ac:dyDescent="0.35">
@@ -6387,10 +6487,10 @@
         <v>335</v>
       </c>
       <c r="D248" s="17" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="E248" s="8" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="G248" t="s">
         <v>449</v>
@@ -6399,7 +6499,7 @@
         <v>450</v>
       </c>
       <c r="K248" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="249" spans="1:11" x14ac:dyDescent="0.35">
@@ -6420,7 +6520,7 @@
       </c>
       <c r="D250" s="18"/>
       <c r="E250" s="8" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="G250" t="s">
         <v>449</v>
@@ -6429,7 +6529,7 @@
         <v>450</v>
       </c>
       <c r="K250" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="251" spans="1:11" x14ac:dyDescent="0.35">
@@ -6474,7 +6574,7 @@
       </c>
       <c r="D254" s="18"/>
       <c r="E254" s="8" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="G254" t="s">
         <v>449</v>
@@ -6483,10 +6583,10 @@
         <v>450</v>
       </c>
       <c r="I254" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="K254" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="255" spans="1:11" x14ac:dyDescent="0.35">
@@ -6676,10 +6776,10 @@
       </c>
       <c r="D270" s="18"/>
       <c r="G270" t="s">
+        <v>569</v>
+      </c>
+      <c r="I270" s="2" t="s">
         <v>570</v>
-      </c>
-      <c r="I270" s="2" t="s">
-        <v>571</v>
       </c>
     </row>
     <row r="271" spans="1:9" x14ac:dyDescent="0.35">
@@ -6694,7 +6794,7 @@
         <v>73</v>
       </c>
       <c r="I271" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="272" spans="1:9" x14ac:dyDescent="0.35">
@@ -6703,7 +6803,7 @@
       </c>
       <c r="D272" s="18"/>
       <c r="G272" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="273" spans="1:8" x14ac:dyDescent="0.35">
@@ -6724,7 +6824,7 @@
       </c>
       <c r="D274" s="18"/>
       <c r="G274" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="275" spans="1:8" x14ac:dyDescent="0.35">
@@ -6745,7 +6845,7 @@
       </c>
       <c r="D276" s="18"/>
       <c r="G276" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="277" spans="1:8" x14ac:dyDescent="0.35">
@@ -6766,7 +6866,7 @@
       </c>
       <c r="D278" s="18"/>
       <c r="G278" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="279" spans="1:8" x14ac:dyDescent="0.35">
@@ -6787,7 +6887,7 @@
       </c>
       <c r="D280" s="18"/>
       <c r="G280" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="281" spans="1:8" x14ac:dyDescent="0.35">
@@ -6808,7 +6908,7 @@
       </c>
       <c r="D282" s="18"/>
       <c r="G282" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="283" spans="1:8" x14ac:dyDescent="0.35">
@@ -6829,7 +6929,7 @@
       </c>
       <c r="D284" s="18"/>
       <c r="G284" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="285" spans="1:8" x14ac:dyDescent="0.35">
@@ -6875,7 +6975,7 @@
         <v>449</v>
       </c>
       <c r="H288" s="3" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="289" spans="1:11" x14ac:dyDescent="0.35">
@@ -6883,10 +6983,10 @@
         <v>374</v>
       </c>
       <c r="D289" s="17" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="E289" s="8" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="G289" t="s">
         <v>449</v>
@@ -6895,7 +6995,7 @@
         <v>450</v>
       </c>
       <c r="K289" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="290" spans="1:11" x14ac:dyDescent="0.35">
@@ -6916,7 +7016,7 @@
       </c>
       <c r="D291" s="18"/>
       <c r="E291" s="8" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="G291" t="s">
         <v>449</v>
@@ -6925,7 +7025,7 @@
         <v>450</v>
       </c>
       <c r="K291" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="292" spans="1:11" x14ac:dyDescent="0.35">
@@ -6970,7 +7070,7 @@
       </c>
       <c r="D295" s="18"/>
       <c r="E295" s="8" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="G295" t="s">
         <v>449</v>
@@ -6979,10 +7079,10 @@
         <v>450</v>
       </c>
       <c r="I295" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="K295" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="296" spans="1:11" x14ac:dyDescent="0.35">
@@ -7148,7 +7248,7 @@
       </c>
       <c r="D309" s="18"/>
       <c r="G309" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="310" spans="1:8" x14ac:dyDescent="0.35">
@@ -7169,7 +7269,7 @@
       </c>
       <c r="D311" s="18"/>
       <c r="G311" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="312" spans="1:8" x14ac:dyDescent="0.35">
@@ -7190,7 +7290,7 @@
       </c>
       <c r="D313" s="18"/>
       <c r="G313" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="314" spans="1:8" x14ac:dyDescent="0.35">
@@ -7211,7 +7311,7 @@
       </c>
       <c r="D315" s="18"/>
       <c r="G315" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="316" spans="1:8" x14ac:dyDescent="0.35">
@@ -7232,7 +7332,7 @@
       </c>
       <c r="D317" s="18"/>
       <c r="G317" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="318" spans="1:8" x14ac:dyDescent="0.35">
@@ -7253,7 +7353,7 @@
       </c>
       <c r="D319" s="18"/>
       <c r="G319" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="320" spans="1:8" x14ac:dyDescent="0.35">
@@ -7274,7 +7374,7 @@
       </c>
       <c r="D321" s="18"/>
       <c r="G321" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="322" spans="1:11" x14ac:dyDescent="0.35">
@@ -7320,7 +7420,7 @@
         <v>449</v>
       </c>
       <c r="H325" s="3" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="326" spans="1:11" x14ac:dyDescent="0.35">
@@ -7328,10 +7428,10 @@
         <v>397</v>
       </c>
       <c r="D326" s="17" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="E326" s="8" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="G326" t="s">
         <v>449</v>
@@ -7340,7 +7440,7 @@
         <v>450</v>
       </c>
       <c r="K326" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="327" spans="1:11" x14ac:dyDescent="0.35">
@@ -7361,7 +7461,7 @@
       </c>
       <c r="D328" s="18"/>
       <c r="E328" s="8" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="G328" t="s">
         <v>449</v>
@@ -7370,7 +7470,7 @@
         <v>450</v>
       </c>
       <c r="K328" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="329" spans="1:11" x14ac:dyDescent="0.35">
@@ -7537,28 +7637,11 @@
         <v>449</v>
       </c>
       <c r="H342" s="3" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="D132:D138"/>
-    <mergeCell ref="D326:D342"/>
-    <mergeCell ref="D139:D148"/>
-    <mergeCell ref="D149:D158"/>
-    <mergeCell ref="D159:D167"/>
-    <mergeCell ref="D168:D176"/>
-    <mergeCell ref="D177:D185"/>
-    <mergeCell ref="D2:D7"/>
-    <mergeCell ref="D8:D11"/>
-    <mergeCell ref="D12:D15"/>
-    <mergeCell ref="D16:D19"/>
-    <mergeCell ref="D20:D23"/>
-    <mergeCell ref="D24:D27"/>
-    <mergeCell ref="D28:D31"/>
-    <mergeCell ref="D32:D35"/>
-    <mergeCell ref="D36:D39"/>
-    <mergeCell ref="D40:D53"/>
     <mergeCell ref="D54:D69"/>
     <mergeCell ref="D248:D288"/>
     <mergeCell ref="D289:D325"/>
@@ -7575,32 +7658,54 @@
     <mergeCell ref="D105:D113"/>
     <mergeCell ref="D114:D122"/>
     <mergeCell ref="D123:D131"/>
+    <mergeCell ref="D24:D27"/>
+    <mergeCell ref="D28:D31"/>
+    <mergeCell ref="D32:D35"/>
+    <mergeCell ref="D36:D39"/>
+    <mergeCell ref="D40:D53"/>
+    <mergeCell ref="D2:D7"/>
+    <mergeCell ref="D8:D11"/>
+    <mergeCell ref="D12:D15"/>
+    <mergeCell ref="D16:D19"/>
+    <mergeCell ref="D20:D23"/>
+    <mergeCell ref="D132:D138"/>
+    <mergeCell ref="D326:D342"/>
+    <mergeCell ref="D139:D148"/>
+    <mergeCell ref="D149:D158"/>
+    <mergeCell ref="D159:D167"/>
+    <mergeCell ref="D168:D176"/>
+    <mergeCell ref="D177:D185"/>
   </mergeCells>
   <conditionalFormatting sqref="E82">
-    <cfRule type="duplicateValues" dxfId="8" priority="4"/>
-    <cfRule type="duplicateValues" dxfId="7" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F20:F27">
-    <cfRule type="duplicateValues" dxfId="6" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F32:F35">
-    <cfRule type="duplicateValues" dxfId="5" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F343:F1048576 F8:F56 F58:F134 F136:F159 F162:F325 E2:E7 F1 G218:H218">
-    <cfRule type="duplicateValues" dxfId="4" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F343:F1048576 F99:F134 F136:F150 F158:F159 F162:F325 F8:F19 E2:E7 F1 F28:F31 F36:F56 F58:F96 G218:H218">
-    <cfRule type="duplicateValues" dxfId="3" priority="67"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="68"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K7">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="2" operator="equal">
       <formula>"Add to practice data and cleaned data"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="3" operator="equal">
       <formula>"Add to practice data"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="4" operator="equal">
       <formula>"Add to cleaned data"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1:H1048576">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="routine">
+      <formula>NOT(ISERROR(SEARCH("routine",H1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>